<commit_message>
csv reader is working
</commit_message>
<xml_diff>
--- a/makePlots/gain_means_norm_by_xtal22.xlsx
+++ b/makePlots/gain_means_norm_by_xtal22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/gain_corrections/makePlots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF440F6-CA58-D84E-951E-C95950D0EC18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4903CBEB-EE7C-424F-8B07-128636BE86DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15900" xr2:uid="{FAD6998E-460B-B541-975C-629B8782B503}"/>
   </bookViews>
@@ -31,26 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>St13</t>
-  </si>
-  <si>
-    <t>xtal_full</t>
-  </si>
-  <si>
-    <t>Xtal</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>St19</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC65671-884D-B640-B34E-10751AEA40DD}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C90"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,1068 +408,1180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.82920025900000005</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1.9196339579999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>1.472927401</v>
+        <v>0.82920025900000005</v>
       </c>
       <c r="C5" s="2">
-        <v>0.59369164500000005</v>
+        <v>1.9196339579999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.89371501900000005</v>
+        <v>1.472927401</v>
       </c>
       <c r="C6" s="2">
-        <v>6.7245869999999998E-3</v>
+        <v>0.59369164500000005</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.88080256999999995</v>
+        <v>0.89371501900000005</v>
       </c>
       <c r="C7" s="2">
-        <v>7.8895900000000001E-3</v>
+        <v>6.7245869999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.80652037700000001</v>
+        <v>0.88080256999999995</v>
       </c>
       <c r="C8" s="2">
-        <v>5.7784910000000002E-3</v>
+        <v>7.8895900000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.25425835000000002</v>
+        <v>0.80652037700000001</v>
       </c>
       <c r="C9" s="2">
-        <v>2.283425276</v>
+        <v>5.7784910000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.95266008000000002</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>3.6523910000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.96126265399999999</v>
+        <v>0.25425835000000002</v>
       </c>
       <c r="C11" s="2">
-        <v>1.829224E-3</v>
+        <v>2.283425276</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.94890182099999998</v>
+        <v>0.95266008000000002</v>
       </c>
       <c r="C12" s="2">
-        <v>1.174088E-3</v>
+        <v>3.6523910000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.93661271700000004</v>
+        <v>0.96126265399999999</v>
       </c>
       <c r="C13" s="2">
-        <v>9.1415099999999998E-4</v>
+        <v>1.829224E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.97307793300000001</v>
+        <v>0.94890182099999998</v>
       </c>
       <c r="C14" s="2">
-        <v>9.5699100000000003E-4</v>
+        <v>1.174088E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.94729243699999999</v>
+        <v>0.93661271700000004</v>
       </c>
       <c r="C15" s="2">
-        <v>9.0044699999999997E-4</v>
+        <v>9.1415099999999998E-4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.88321007900000004</v>
+        <v>0.97307793300000001</v>
       </c>
       <c r="C16" s="2">
-        <v>1.5525300000000001E-3</v>
+        <v>9.5699100000000003E-4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>9.6637772999999996E-2</v>
+        <v>0.94729243699999999</v>
       </c>
       <c r="C17" s="2">
-        <v>2.5867713330000002</v>
+        <v>9.0044699999999997E-4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.96175264199999999</v>
+        <v>0.88321007900000004</v>
       </c>
       <c r="C18" s="2">
-        <v>4.2649869999999996E-3</v>
+        <v>1.5525300000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.98036814800000005</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>1.423314E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>9.6637772999999996E-2</v>
       </c>
       <c r="C20" s="2">
-        <v>9.7727100000000004E-4</v>
+        <v>2.5867713330000002</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.91521387700000001</v>
+        <v>0.96175264199999999</v>
       </c>
       <c r="C21" s="2">
-        <v>8.9298000000000003E-4</v>
+        <v>4.2649869999999996E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.93437998799999999</v>
+        <v>0.98036814800000005</v>
       </c>
       <c r="C22" s="2">
-        <v>8.2986500000000005E-4</v>
+        <v>1.423314E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.97420035999999999</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2">
-        <v>8.5642300000000004E-4</v>
+        <v>9.7727100000000004E-4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.87152916700000005</v>
+        <v>0.91521387700000001</v>
       </c>
       <c r="C24" s="2">
-        <v>1.5363530000000001E-3</v>
+        <v>8.9298000000000003E-4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.45528883999999997</v>
+        <v>0.93437998799999999</v>
       </c>
       <c r="C25" s="2">
-        <v>0.22518661700000001</v>
+        <v>8.2986500000000005E-4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.95183467700000002</v>
+        <v>0.97420035999999999</v>
       </c>
       <c r="C26" s="2">
-        <v>2.9761420000000002E-3</v>
+        <v>8.5642300000000004E-4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.97815663500000005</v>
+        <v>0.87152916700000005</v>
       </c>
       <c r="C27" s="2">
-        <v>1.3677959999999999E-3</v>
+        <v>1.5363530000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2">
-        <v>0.98822007999999995</v>
+        <v>0.45528883999999997</v>
       </c>
       <c r="C28" s="2">
-        <v>9.9478600000000011E-4</v>
+        <v>0.22518661700000001</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>1.0156775979999999</v>
+        <v>0</v>
       </c>
       <c r="C29" s="2">
-        <v>1.0515050000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.98598937200000003</v>
+        <v>0.95183467700000002</v>
       </c>
       <c r="C30" s="2">
-        <v>8.8562199999999997E-4</v>
+        <v>2.9761420000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.98780081200000003</v>
+        <v>0.97815663500000005</v>
       </c>
       <c r="C31" s="2">
-        <v>9.4091699999999999E-4</v>
+        <v>1.3677959999999999E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.90239841600000004</v>
+        <v>0.98822007999999995</v>
       </c>
       <c r="C32" s="2">
-        <v>1.3651150000000001E-3</v>
+        <v>9.9478600000000011E-4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>9.4455557999999995E-2</v>
+        <v>1.0156775979999999</v>
       </c>
       <c r="C33" s="2">
-        <v>4.5461205070000004</v>
+        <v>1.0515050000000001E-3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>1.3370774480000001</v>
+        <v>0.98598937200000003</v>
       </c>
       <c r="C34" s="2">
-        <v>0.37771930100000001</v>
+        <v>8.8562199999999997E-4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.96292861299999999</v>
+        <v>0.98780081200000003</v>
       </c>
       <c r="C35" s="2">
-        <v>2.0554850000000001E-3</v>
+        <v>9.4091699999999999E-4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.97531874500000004</v>
+        <v>0.90239841600000004</v>
       </c>
       <c r="C36" s="2">
-        <v>1.2077489999999999E-3</v>
+        <v>1.3651150000000001E-3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.97421349300000004</v>
+        <v>0</v>
       </c>
       <c r="C37" s="2">
-        <v>1.048003E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.95886120699999999</v>
+        <v>9.4455557999999995E-2</v>
       </c>
       <c r="C38" s="2">
-        <v>9.2863199999999998E-4</v>
+        <v>4.5461205070000004</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.95687195700000005</v>
+        <v>1.3370774480000001</v>
       </c>
       <c r="C39" s="2">
-        <v>9.5569899999999996E-4</v>
+        <v>0.37771930100000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>0.90665777599999997</v>
+        <v>0.96292861299999999</v>
       </c>
       <c r="C40" s="2">
-        <v>1.347642E-3</v>
+        <v>2.0554850000000001E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>0.90649107900000003</v>
+        <v>0.97531874500000004</v>
       </c>
       <c r="C41" s="2">
-        <v>1.825020818</v>
+        <v>1.2077489999999999E-3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>1.1418520539999999</v>
+        <v>0.97421349300000004</v>
       </c>
       <c r="C42" s="2">
-        <v>0.68724156800000002</v>
+        <v>1.048003E-3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>1.1945303190000001</v>
+        <v>0.95886120699999999</v>
       </c>
       <c r="C43" s="2">
-        <v>0.441172905</v>
+        <v>9.2863199999999998E-4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>0.84048513899999999</v>
+        <v>0.95687195700000005</v>
       </c>
       <c r="C44" s="2">
-        <v>5.2774550000000003E-3</v>
+        <v>9.5569899999999996E-4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>1.161805177</v>
+        <v>0.90665777599999997</v>
       </c>
       <c r="C45" s="2">
-        <v>0.270659492</v>
+        <v>1.347642E-3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>4</v>
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>0.87976157399999999</v>
+        <v>0</v>
       </c>
       <c r="C49" s="2">
-        <v>2.0873458309999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>0.805967722</v>
+        <v>0.90649107900000003</v>
       </c>
       <c r="C50" s="2">
-        <v>0.73028182799999997</v>
+        <v>1.825020818</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>0.91396458999999997</v>
+        <v>1.1418520539999999</v>
       </c>
       <c r="C51" s="2">
-        <v>7.8198539999999993E-3</v>
+        <v>0.68724156800000002</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>0.896760538</v>
+        <v>1.1945303190000001</v>
       </c>
       <c r="C52" s="2">
-        <v>4.364176E-3</v>
+        <v>0.441172905</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>0.87095900800000003</v>
+        <v>0.84048513899999999</v>
       </c>
       <c r="C53" s="2">
-        <v>0.17097875700000001</v>
+        <v>5.2774550000000003E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>0.89682317600000006</v>
+        <v>1.161805177</v>
       </c>
       <c r="C54" s="2">
-        <v>3.880720379</v>
+        <v>0.270659492</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B55" s="2">
-        <v>0.92009496599999996</v>
+        <v>0</v>
       </c>
       <c r="C55" s="2">
-        <v>1.4343905000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B56" s="2">
-        <v>0.95248655100000001</v>
+        <v>0</v>
       </c>
       <c r="C56" s="2">
-        <v>1.699571E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B57" s="2">
-        <v>0.97459550900000003</v>
+        <v>0</v>
       </c>
       <c r="C57" s="2">
-        <v>1.1924150000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B58" s="2">
-        <v>1.0228292880000001</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2">
-        <v>1.140526E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B59" s="2">
-        <v>0.98700174299999999</v>
+        <v>0.87976157399999999</v>
       </c>
       <c r="C59" s="2">
-        <v>9.44698E-4</v>
+        <v>2.0873458309999999</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B60" s="2">
-        <v>0.98376581699999999</v>
+        <v>0.805967722</v>
       </c>
       <c r="C60" s="2">
-        <v>9.2850699999999997E-4</v>
+        <v>0.73028182799999997</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B61" s="2">
-        <v>0.92340464200000005</v>
+        <v>0.91396458999999997</v>
       </c>
       <c r="C61" s="2">
-        <v>1.6657250000000001E-3</v>
+        <v>7.8198539999999993E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B62" s="2">
-        <v>1.1428111030000001</v>
+        <v>0.896760538</v>
       </c>
       <c r="C62" s="2">
-        <v>2.3573531999999999</v>
+        <v>4.364176E-3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B63" s="2">
-        <v>0.92691334299999995</v>
+        <v>0.87095900800000003</v>
       </c>
       <c r="C63" s="2">
-        <v>9.7228369999999998E-3</v>
+        <v>0.17097875700000001</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B64" s="2">
-        <v>0.96280150499999995</v>
+        <v>0.89682317600000006</v>
       </c>
       <c r="C64" s="2">
-        <v>1.3696369999999999E-3</v>
+        <v>3.880720379</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B65" s="2">
-        <v>1</v>
+        <v>0.92009496599999996</v>
       </c>
       <c r="C65" s="2">
-        <v>1.000389E-3</v>
+        <v>1.4343905000000001E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B66" s="2">
-        <v>0.95197838000000001</v>
+        <v>0.95248655100000001</v>
       </c>
       <c r="C66" s="2">
-        <v>8.7030799999999998E-4</v>
+        <v>1.699571E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B67" s="2">
-        <v>0.96294193400000005</v>
+        <v>0.97459550900000003</v>
       </c>
       <c r="C67" s="2">
-        <v>8.6626900000000002E-4</v>
+        <v>1.1924150000000001E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B68" s="2">
-        <v>1.008214583</v>
+        <v>1.0228292880000001</v>
       </c>
       <c r="C68" s="2">
-        <v>8.8613799999999996E-4</v>
+        <v>1.140526E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B69" s="2">
-        <v>0.94198671499999997</v>
+        <v>0.98700174299999999</v>
       </c>
       <c r="C69" s="2">
-        <v>1.559749E-3</v>
+        <v>9.44698E-4</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B70" s="2">
-        <v>0.86874245400000005</v>
+        <v>0.98376581699999999</v>
       </c>
       <c r="C70" s="2">
-        <v>2.9167489820000001</v>
+        <v>9.2850699999999997E-4</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B71" s="2">
-        <v>1.4995337559999999</v>
+        <v>0.92340464200000005</v>
       </c>
       <c r="C71" s="2">
-        <v>0.31583328599999999</v>
+        <v>1.6657250000000001E-3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B72" s="2">
-        <v>0.96899249899999995</v>
+        <v>0</v>
       </c>
       <c r="C72" s="2">
-        <v>1.4886299999999999E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B73" s="2">
-        <v>0.94900916800000001</v>
+        <v>1.1428111030000001</v>
       </c>
       <c r="C73" s="2">
-        <v>1.026758E-3</v>
+        <v>2.3573531999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B74" s="2">
-        <v>0.96933094200000003</v>
+        <v>0.92691334299999995</v>
       </c>
       <c r="C74" s="2">
-        <v>8.6134799999999995E-4</v>
+        <v>9.7228369999999998E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B75" s="2">
-        <v>0.98325562600000005</v>
+        <v>0.96280150499999995</v>
       </c>
       <c r="C75" s="2">
-        <v>8.5702E-4</v>
+        <v>1.3696369999999999E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B76" s="2">
-        <v>0.99092364799999999</v>
+        <v>1</v>
       </c>
       <c r="C76" s="2">
-        <v>8.8567699999999997E-4</v>
+        <v>1.000389E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B77" s="2">
-        <v>0.93480463700000005</v>
+        <v>0.95197838000000001</v>
       </c>
       <c r="C77" s="2">
-        <v>1.3541250000000001E-3</v>
+        <v>8.7030799999999998E-4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B78" s="2">
-        <v>0.70573586200000005</v>
+        <v>0.96294193400000005</v>
       </c>
       <c r="C78" s="2">
-        <v>0.25260269800000001</v>
+        <v>8.6626900000000002E-4</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B79" s="2">
-        <v>0.98285050399999996</v>
+        <v>1.008214583</v>
       </c>
       <c r="C79" s="2">
-        <v>0.12033935</v>
+        <v>8.8613799999999996E-4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B80" s="2">
-        <v>0.95879776699999997</v>
+        <v>0.94198671499999997</v>
       </c>
       <c r="C80" s="2">
-        <v>2.3337950000000001E-3</v>
+        <v>1.559749E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B81" s="2">
-        <v>0.91803702700000001</v>
+        <v>0.86874245400000005</v>
       </c>
       <c r="C81" s="2">
-        <v>1.0571210000000001E-3</v>
+        <v>2.9167489820000001</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B82" s="2">
-        <v>0.98342232200000002</v>
+        <v>0</v>
       </c>
       <c r="C82" s="2">
-        <v>1.0903600000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B83" s="2">
-        <v>0.98740787500000005</v>
+        <v>1.4995337559999999</v>
       </c>
       <c r="C83" s="2">
-        <v>1.0054759999999999E-3</v>
+        <v>0.31583328599999999</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B84" s="2">
-        <v>0.92828126200000005</v>
+        <v>0.96899249899999995</v>
       </c>
       <c r="C84" s="2">
-        <v>9.7592299999999996E-4</v>
+        <v>1.4886299999999999E-3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B85" s="2">
-        <v>0.91397873399999996</v>
+        <v>0.94900916800000001</v>
       </c>
       <c r="C85" s="2">
-        <v>1.5748750000000001E-3</v>
+        <v>1.026758E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B86" s="2">
-        <v>0.872676483</v>
+        <v>0.96933094200000003</v>
       </c>
       <c r="C86" s="2">
-        <v>1.9917663130000001</v>
+        <v>8.6134799999999995E-4</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B87" s="2">
-        <v>0.97082413599999995</v>
+        <v>0.98325562600000005</v>
       </c>
       <c r="C87" s="2">
-        <v>1.2071216469999999</v>
+        <v>8.5702E-4</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B88" s="2">
-        <v>0.84780238900000005</v>
+        <v>0.99092364799999999</v>
       </c>
       <c r="C88" s="2">
-        <v>4.38056E-2</v>
+        <v>8.8567699999999997E-4</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B89" s="2">
-        <v>0.84336322100000005</v>
+        <v>0.93480463700000005</v>
       </c>
       <c r="C89" s="2">
-        <v>7.2520060000000001E-3</v>
+        <v>1.3541250000000001E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
+        <v>37</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.70573586200000005</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.25260269800000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>38</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.98285050399999996</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.12033935</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>39</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.95879776699999997</v>
+      </c>
+      <c r="C92" s="2">
+        <v>2.3337950000000001E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>40</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.91803702700000001</v>
+      </c>
+      <c r="C93" s="2">
+        <v>1.0571210000000001E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>41</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.98342232200000002</v>
+      </c>
+      <c r="C94" s="2">
+        <v>1.0903600000000001E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>42</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.98740787500000005</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1.0054759999999999E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>43</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.92828126200000005</v>
+      </c>
+      <c r="C96" s="2">
+        <v>9.7592299999999996E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>44</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.91397873399999996</v>
+      </c>
+      <c r="C97" s="2">
+        <v>1.5748750000000001E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>45</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>46</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>47</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>48</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>49</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.872676483</v>
+      </c>
+      <c r="C102" s="2">
+        <v>1.9917663130000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>50</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.97082413599999995</v>
+      </c>
+      <c r="C103" s="2">
+        <v>1.2071216469999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>51</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.84780238900000005</v>
+      </c>
+      <c r="C104" s="2">
+        <v>4.38056E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>52</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.84336322100000005</v>
+      </c>
+      <c r="C105" s="2">
+        <v>7.2520060000000001E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
         <v>53</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B106" s="2">
         <v>0.45530472599999999</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C106" s="2">
         <v>0.468431394</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
@@ -1615,6 +1708,86 @@
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
     </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="2"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>